<commit_message>
update result 20201127 & update plane 20201130
</commit_message>
<xml_diff>
--- a/20201127.xlsx
+++ b/20201127.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AD4E8E-42DB-4981-AAC1-3134865AA18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90254D1A-BBF9-4BBD-AADC-263B2BFC8096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>일</t>
   </si>
@@ -203,7 +203,12 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>1. 빨래</t>
+    <t>F7 초기 UI통합(그리는 시간 줄이기 위해)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 빨래
+2. NCT세트 피앤이로부터 전달 받으면 사설IP, 외부IP에 따라 타임아웃 적용이 다르게 되던 현상 테스트 할 것</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
@@ -214,8 +219,13 @@
   -&gt; 설정한 타임아웃 적용되도록 수정 (w5100s init타임 후 설정해야함)
  - DHCP 보완
   -&gt; 기존 10회동안만 요청하던 dhcp를 할당받기 전까지 계속 요청하도록 변경
- - 5v 풀업 점핑 4ea
-  -&gt; 금일부터 5v풀업 점핑보드를 최종으로 선정, 이후 문제 시 롤백</t>
+ - 5v 풀업 점핑 5ea
+  -&gt; 금일부터 5v풀업 점핑보드를 최종으로 선정, 이후 문제 시 롤백
+ - 납품
+  -&gt;5ea (3ea는 26일자버젼 MAC : 80~82, 2ea는 27일자버젼(DHCP수정), MAC : 83~84)
+ - MAC구입?
+  -&gt; 4096ea : 550달러, 16,777,216ea : 1,650달러
+  -&gt; MAC이 내장된 EEPROM타입 구입 : microchip 약 2800원, ICbanQ 약 12000원</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -389,7 +399,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,8 +612,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -872,7 +900,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -885,71 +913,68 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1484,7 +1509,7 @@
   <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="C3:G23"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1520,7 +1545,7 @@
       <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="4"/>
       <c r="I2" t="s">
         <v>15</v>
       </c>
@@ -1538,23 +1563,23 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="4"/>
       <c r="I3" t="s">
         <v>13</v>
       </c>
@@ -1566,13 +1591,13 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="8"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
       <c r="I4" t="s">
         <v>11</v>
       </c>
@@ -1581,13 +1606,13 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="8"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
       <c r="I5" t="s">
         <v>12</v>
       </c>
@@ -1596,13 +1621,13 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="8"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4"/>
       <c r="I6" t="s">
         <v>10</v>
       </c>
@@ -1611,13 +1636,13 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="8"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
       <c r="I7" t="s">
         <v>8</v>
       </c>
@@ -1630,13 +1655,13 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="8"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4"/>
       <c r="I8" t="s">
         <v>4</v>
       </c>
@@ -1645,199 +1670,199 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="8"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="8"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="8"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="8"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="8"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="8"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="8"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="8"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="8"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="8"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="8"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="8"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>

</xml_diff>